<commit_message>
Added costs for certificate
</commit_message>
<xml_diff>
--- a/doc/abrechnung_intern/kosten.xlsx
+++ b/doc/abrechnung_intern/kosten.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -54,9 +54,6 @@
     <t>09.09.2015 - 08.09.2016</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Server</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>22.03.2016 - 21.06.2016</t>
+  </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>12.10.2015 - 12.10.3016</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +105,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,8 +125,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -335,12 +350,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -363,10 +420,33 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -379,9 +459,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -419,7 +499,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -491,7 +571,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -665,13 +745,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -724,7 +804,7 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="13"/>
       <c r="I2" s="14"/>
     </row>
@@ -733,27 +813,27 @@
         <v>9</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" s="12">
-        <v>35</v>
+        <v>35.29</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D7" si="0">C3/5</f>
-        <v>7</v>
+        <v>7.0579999999999998</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="15"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="12">
         <v>27.2</v>
@@ -764,16 +844,16 @@
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="12">
         <v>27.2</v>
@@ -784,16 +864,16 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="12">
         <v>27.2</v>
@@ -804,16 +884,16 @@
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="19">
         <v>27.2</v>
@@ -824,11 +904,69 @@
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="20"/>
       <c r="I7" s="21"/>
     </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="23">
+        <f>SUM(C2:C7)</f>
+        <v>158.20999999999998</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="35">
+        <f>SUM(D2:D7)</f>
+        <v>31.641999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="29"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="29"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="G20:H20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -840,7 +978,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -852,7 +990,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>